<commit_message>
Xlsx adjusted to included a interger Id column. Done so that Clip model does not run into a processing issue. Jsonify script also adjusted to handle an additional column when converting into a tsv.
</commit_message>
<xml_diff>
--- a/data/xlsx/Ad_Final cleaned 14 scenes 9.12.24.xlsx
+++ b/data/xlsx/Ad_Final cleaned 14 scenes 9.12.24.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28816"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bigimac/Box/SanockiLab on Box/2023 PN 8 scenes + Priming (+:-)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9254811-141C-4F4F-BB41-302DAFD2A58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{09A45002-03FD-4F67-B6AA-69501B5866E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3700" yWindow="1020" windowWidth="41080" windowHeight="26520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="725">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="726">
+  <si>
+    <t>Int_id</t>
+  </si>
   <si>
     <t>orig ID</t>
   </si>
@@ -3534,7 +3537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3585,25 +3588,11 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3967,40 +3956,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q58"/>
+  <dimension ref="A1:R58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="132" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C5" sqref="C5"/>
+      <pane xSplit="2" topLeftCell="C30" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16" width="168.85546875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="168.85546875" style="8" customWidth="1"/>
-    <col min="18" max="22" width="168.85546875" style="2" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="17" width="168.85546875" style="2" customWidth="1"/>
+    <col min="18" max="18" width="168.85546875" style="8" customWidth="1"/>
+    <col min="19" max="23" width="168.85546875" style="2" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:17">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="6" t="s">
@@ -4033,27 +4022,30 @@
       <c r="P1" s="6" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="3" t="s">
-        <v>16</v>
+    <row r="2" spans="1:17">
+      <c r="A2" s="2">
+        <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="8" t="s">
         <v>22</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -4065,10 +4057,10 @@
       <c r="J2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="L2" s="21" t="s">
         <v>27</v>
       </c>
       <c r="M2" s="22" t="s">
@@ -4077,33 +4069,36 @@
       <c r="N2" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="23" t="s">
+      <c r="O2" s="22" t="s">
         <v>30</v>
       </c>
       <c r="P2" s="23" t="s">
         <v>31</v>
       </c>
+      <c r="Q2" s="23" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="3" spans="1:16">
-      <c r="A3" s="3" t="s">
-        <v>32</v>
+    <row r="3" spans="1:17">
+      <c r="A3" s="2">
+        <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="8" t="s">
         <v>38</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -4112,13 +4107,13 @@
       <c r="I3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="K3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="L3" s="21" t="s">
         <v>43</v>
       </c>
       <c r="M3" s="22" t="s">
@@ -4127,33 +4122,36 @@
       <c r="N3" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="O3" s="23" t="s">
+      <c r="O3" s="22" t="s">
         <v>46</v>
       </c>
       <c r="P3" s="23" t="s">
         <v>47</v>
       </c>
+      <c r="Q3" s="23" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="3" t="s">
-        <v>48</v>
+    <row r="4" spans="1:17">
+      <c r="A4" s="2">
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="8" t="s">
         <v>54</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -4165,45 +4163,48 @@
       <c r="J4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="K4" s="21" t="s">
+      <c r="K4" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="L4" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="M4" s="22" t="s">
+      <c r="M4" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="O4" s="23" t="s">
+      <c r="O4" s="25" t="s">
         <v>62</v>
       </c>
       <c r="P4" s="23" t="s">
         <v>63</v>
       </c>
+      <c r="Q4" s="23" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="3" t="s">
-        <v>64</v>
+    <row r="5" spans="1:17">
+      <c r="A5" s="2">
+        <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="8" t="s">
         <v>70</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -4212,48 +4213,51 @@
       <c r="I5" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="K5" s="21" t="s">
+      <c r="K5" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="L5" s="22" t="s">
+      <c r="L5" s="21" t="s">
         <v>75</v>
       </c>
       <c r="M5" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="N5" s="24" t="s">
+      <c r="N5" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="O5" s="23" t="s">
+      <c r="O5" s="24" t="s">
         <v>78</v>
       </c>
       <c r="P5" s="23" t="s">
         <v>79</v>
       </c>
+      <c r="Q5" s="23" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="3" t="s">
-        <v>80</v>
+    <row r="6" spans="1:17">
+      <c r="A6" s="2">
+        <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="8" t="s">
         <v>86</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -4265,10 +4269,10 @@
       <c r="J6" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="K6" s="21" t="s">
+      <c r="K6" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="L6" s="22" t="s">
+      <c r="L6" s="21" t="s">
         <v>91</v>
       </c>
       <c r="M6" s="22" t="s">
@@ -4277,33 +4281,36 @@
       <c r="N6" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="O6" s="23" t="s">
+      <c r="O6" s="22" t="s">
         <v>94</v>
       </c>
       <c r="P6" s="23" t="s">
         <v>95</v>
       </c>
+      <c r="Q6" s="23" t="s">
+        <v>96</v>
+      </c>
     </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="3" t="s">
-        <v>96</v>
+    <row r="7" spans="1:17">
+      <c r="A7" s="2">
+        <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="8" t="s">
         <v>102</v>
       </c>
       <c r="H7" s="2" t="s">
@@ -4312,48 +4319,51 @@
       <c r="I7" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="K7" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="L7" s="22" t="s">
+      <c r="L7" s="21" t="s">
         <v>107</v>
       </c>
       <c r="M7" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="N7" s="26" t="s">
+      <c r="N7" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="O7" s="23" t="s">
+      <c r="O7" s="26" t="s">
         <v>110</v>
       </c>
       <c r="P7" s="23" t="s">
         <v>111</v>
       </c>
+      <c r="Q7" s="23" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="3" t="s">
-        <v>112</v>
+    <row r="8" spans="1:17">
+      <c r="A8" s="2">
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="8" t="s">
         <v>118</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -4365,10 +4375,10 @@
       <c r="J8" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K8" s="21" t="s">
+      <c r="K8" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="L8" s="22" t="s">
+      <c r="L8" s="21" t="s">
         <v>123</v>
       </c>
       <c r="M8" s="22" t="s">
@@ -4377,83 +4387,89 @@
       <c r="N8" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="O8" s="23" t="s">
+      <c r="O8" s="22" t="s">
         <v>126</v>
       </c>
       <c r="P8" s="23" t="s">
         <v>127</v>
       </c>
+      <c r="Q8" s="23" t="s">
+        <v>128</v>
+      </c>
     </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="3" t="s">
-        <v>128</v>
+    <row r="9" spans="1:17">
+      <c r="A9" s="2">
+        <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="12" t="s">
         <v>136</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="K9" s="21" t="s">
+      <c r="K9" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="L9" s="24" t="s">
+      <c r="L9" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="M9" s="22" t="s">
+      <c r="M9" s="24" t="s">
         <v>140</v>
       </c>
       <c r="N9" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="O9" s="23" t="s">
+      <c r="O9" s="22" t="s">
         <v>142</v>
       </c>
       <c r="P9" s="23" t="s">
         <v>143</v>
       </c>
+      <c r="Q9" s="23" t="s">
+        <v>144</v>
+      </c>
     </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="3" t="s">
-        <v>144</v>
+    <row r="10" spans="1:17">
+      <c r="A10" s="2">
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="8" t="s">
         <v>150</v>
       </c>
       <c r="H10" s="2" t="s">
@@ -4465,45 +4481,48 @@
       <c r="J10" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="K10" s="21" t="s">
+      <c r="K10" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="L10" s="22" t="s">
+      <c r="L10" s="21" t="s">
         <v>155</v>
       </c>
       <c r="M10" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="N10" s="26" t="s">
+      <c r="N10" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="O10" s="23" t="s">
+      <c r="O10" s="26" t="s">
         <v>158</v>
       </c>
       <c r="P10" s="23" t="s">
         <v>159</v>
       </c>
+      <c r="Q10" s="23" t="s">
+        <v>160</v>
+      </c>
     </row>
-    <row r="11" spans="1:16">
-      <c r="A11" s="3" t="s">
-        <v>160</v>
+    <row r="11" spans="1:17">
+      <c r="A11" s="2">
+        <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="8" t="s">
         <v>166</v>
       </c>
       <c r="H11" s="2" t="s">
@@ -4512,13 +4531,13 @@
       <c r="I11" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="J11" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="K11" s="21" t="s">
+      <c r="K11" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="L11" s="22" t="s">
+      <c r="L11" s="21" t="s">
         <v>171</v>
       </c>
       <c r="M11" s="22" t="s">
@@ -4527,33 +4546,36 @@
       <c r="N11" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="O11" s="23" t="s">
+      <c r="O11" s="22" t="s">
         <v>174</v>
       </c>
       <c r="P11" s="23" t="s">
         <v>175</v>
       </c>
+      <c r="Q11" s="23" t="s">
+        <v>176</v>
+      </c>
     </row>
-    <row r="12" spans="1:16">
-      <c r="A12" s="3" t="s">
-        <v>176</v>
+    <row r="12" spans="1:17">
+      <c r="A12" s="2">
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="8" t="s">
         <v>182</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -4565,45 +4587,48 @@
       <c r="J12" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="K12" s="21" t="s">
+      <c r="K12" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="L12" s="22" t="s">
+      <c r="L12" s="21" t="s">
         <v>187</v>
       </c>
       <c r="M12" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="N12" s="26" t="s">
+      <c r="N12" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="O12" s="27" t="s">
+      <c r="O12" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="P12" s="23" t="s">
+      <c r="P12" s="27" t="s">
         <v>191</v>
       </c>
+      <c r="Q12" s="23" t="s">
+        <v>192</v>
+      </c>
     </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="3" t="s">
-        <v>192</v>
+    <row r="13" spans="1:17">
+      <c r="A13" s="2">
+        <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="8" t="s">
         <v>198</v>
       </c>
       <c r="H13" s="2" t="s">
@@ -4615,45 +4640,48 @@
       <c r="J13" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="K13" s="21" t="s">
+      <c r="K13" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="L13" s="22" t="s">
+      <c r="L13" s="21" t="s">
         <v>203</v>
       </c>
       <c r="M13" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="N13" s="24" t="s">
+      <c r="N13" s="22" t="s">
         <v>205</v>
       </c>
-      <c r="O13" s="23" t="s">
+      <c r="O13" s="24" t="s">
         <v>206</v>
       </c>
       <c r="P13" s="23" t="s">
         <v>207</v>
       </c>
+      <c r="Q13" s="23" t="s">
+        <v>208</v>
+      </c>
     </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="3" t="s">
-        <v>208</v>
+    <row r="14" spans="1:17">
+      <c r="A14" s="2">
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="8" t="s">
         <v>214</v>
       </c>
       <c r="H14" s="2" t="s">
@@ -4662,113 +4690,119 @@
       <c r="I14" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="J14" s="20" t="s">
+      <c r="J14" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="K14" s="21" t="s">
+      <c r="K14" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="L14" s="22" t="s">
+      <c r="L14" s="21" t="s">
         <v>219</v>
       </c>
-      <c r="M14" s="24" t="s">
+      <c r="M14" s="22" t="s">
         <v>220</v>
       </c>
       <c r="N14" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="O14" s="23" t="s">
+      <c r="O14" s="24" t="s">
         <v>222</v>
       </c>
       <c r="P14" s="23" t="s">
         <v>223</v>
       </c>
+      <c r="Q14" s="23" t="s">
+        <v>224</v>
+      </c>
     </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="3" t="s">
-        <v>224</v>
+    <row r="15" spans="1:17">
+      <c r="A15" s="2">
+        <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="8" t="s">
         <v>230</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="J15" s="15" t="s">
+      <c r="J15" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="K15" s="21" t="s">
+      <c r="K15" s="15" t="s">
         <v>234</v>
       </c>
-      <c r="L15" s="24" t="s">
+      <c r="L15" s="21" t="s">
         <v>235</v>
       </c>
-      <c r="M15" s="22" t="s">
+      <c r="M15" s="24" t="s">
         <v>236</v>
       </c>
       <c r="N15" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="O15" s="23" t="s">
+      <c r="O15" s="22" t="s">
         <v>238</v>
       </c>
       <c r="P15" s="23" t="s">
         <v>239</v>
       </c>
+      <c r="Q15" s="23" t="s">
+        <v>240</v>
+      </c>
     </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="3" t="s">
-        <v>224</v>
+    <row r="16" spans="1:17">
+      <c r="A16" s="2">
+        <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="C16" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="8" t="s">
         <v>245</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="I16" s="7" t="s">
+      <c r="I16" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="J16" s="15" t="s">
+      <c r="J16" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="K16" s="21" t="s">
+      <c r="K16" s="15" t="s">
         <v>249</v>
       </c>
-      <c r="L16" s="22" t="s">
+      <c r="L16" s="21" t="s">
         <v>250</v>
       </c>
       <c r="M16" s="22" t="s">
@@ -4777,48 +4811,51 @@
       <c r="N16" s="22" t="s">
         <v>252</v>
       </c>
-      <c r="O16" s="23" t="s">
+      <c r="O16" s="22" t="s">
         <v>253</v>
       </c>
       <c r="P16" s="23" t="s">
         <v>254</v>
       </c>
+      <c r="Q16" s="23" t="s">
+        <v>255</v>
+      </c>
     </row>
-    <row r="17" spans="1:16">
-      <c r="A17" s="3" t="s">
-        <v>224</v>
+    <row r="17" spans="1:17">
+      <c r="A17" s="2">
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="C17" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="8" t="s">
         <v>260</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="I17" s="7" t="s">
+      <c r="I17" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="J17" s="19" t="s">
+      <c r="J17" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="K17" s="21" t="s">
+      <c r="K17" s="19" t="s">
         <v>264</v>
       </c>
-      <c r="L17" s="22" t="s">
+      <c r="L17" s="21" t="s">
         <v>265</v>
       </c>
       <c r="M17" s="22" t="s">
@@ -4827,33 +4864,36 @@
       <c r="N17" s="22" t="s">
         <v>267</v>
       </c>
-      <c r="O17" s="28" t="s">
+      <c r="O17" s="22" t="s">
         <v>268</v>
       </c>
-      <c r="P17" s="23" t="s">
+      <c r="P17" s="28" t="s">
         <v>269</v>
       </c>
+      <c r="Q17" s="23" t="s">
+        <v>270</v>
+      </c>
     </row>
-    <row r="18" spans="1:16">
-      <c r="A18" s="3" t="s">
-        <v>270</v>
+    <row r="18" spans="1:17">
+      <c r="A18" s="2">
+        <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="8" t="s">
         <v>276</v>
       </c>
       <c r="H18" s="2" t="s">
@@ -4862,48 +4902,51 @@
       <c r="I18" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="J18" s="10" t="s">
+      <c r="J18" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="K18" s="21" t="s">
+      <c r="K18" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="L18" s="22" t="s">
+      <c r="L18" s="21" t="s">
         <v>281</v>
       </c>
       <c r="M18" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="N18" s="24" t="s">
+      <c r="N18" s="22" t="s">
         <v>283</v>
       </c>
-      <c r="O18" s="23" t="s">
+      <c r="O18" s="24" t="s">
         <v>284</v>
       </c>
       <c r="P18" s="23" t="s">
         <v>285</v>
       </c>
+      <c r="Q18" s="23" t="s">
+        <v>286</v>
+      </c>
     </row>
-    <row r="19" spans="1:16">
-      <c r="A19" s="3" t="s">
-        <v>286</v>
+    <row r="19" spans="1:17">
+      <c r="A19" s="2">
+        <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="8" t="s">
         <v>292</v>
       </c>
       <c r="H19" s="2" t="s">
@@ -4915,10 +4958,10 @@
       <c r="J19" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="K19" s="21" t="s">
+      <c r="K19" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="L19" s="22" t="s">
+      <c r="L19" s="21" t="s">
         <v>297</v>
       </c>
       <c r="M19" s="22" t="s">
@@ -4927,33 +4970,36 @@
       <c r="N19" s="22" t="s">
         <v>299</v>
       </c>
-      <c r="O19" s="23" t="s">
+      <c r="O19" s="22" t="s">
         <v>300</v>
       </c>
       <c r="P19" s="23" t="s">
         <v>301</v>
       </c>
+      <c r="Q19" s="23" t="s">
+        <v>302</v>
+      </c>
     </row>
-    <row r="20" spans="1:16">
-      <c r="A20" s="3" t="s">
-        <v>302</v>
+    <row r="20" spans="1:17">
+      <c r="A20" s="2">
+        <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="12" t="s">
         <v>307</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="8" t="s">
         <v>308</v>
       </c>
       <c r="H20" s="2" t="s">
@@ -4962,13 +5008,13 @@
       <c r="I20" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="J20" s="18" t="s">
+      <c r="J20" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="K20" s="21" t="s">
+      <c r="K20" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="L20" s="22" t="s">
+      <c r="L20" s="21" t="s">
         <v>313</v>
       </c>
       <c r="M20" s="22" t="s">
@@ -4977,33 +5023,36 @@
       <c r="N20" s="22" t="s">
         <v>315</v>
       </c>
-      <c r="O20" s="23" t="s">
+      <c r="O20" s="22" t="s">
         <v>316</v>
       </c>
       <c r="P20" s="23" t="s">
         <v>317</v>
       </c>
+      <c r="Q20" s="23" t="s">
+        <v>318</v>
+      </c>
     </row>
-    <row r="21" spans="1:16">
-      <c r="A21" s="3" t="s">
-        <v>318</v>
+    <row r="21" spans="1:17">
+      <c r="A21" s="2">
+        <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="7" t="s">
         <v>322</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="8" t="s">
         <v>324</v>
       </c>
       <c r="H21" s="2" t="s">
@@ -5012,48 +5061,51 @@
       <c r="I21" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="J21" s="12" t="s">
+      <c r="J21" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="K21" s="21" t="s">
+      <c r="K21" s="12" t="s">
         <v>328</v>
       </c>
-      <c r="L21" s="22" t="s">
+      <c r="L21" s="21" t="s">
         <v>329</v>
       </c>
-      <c r="M21" s="29" t="s">
+      <c r="M21" s="22" t="s">
         <v>330</v>
       </c>
-      <c r="N21" s="24" t="s">
+      <c r="N21" s="29" t="s">
         <v>331</v>
       </c>
-      <c r="O21" s="23" t="s">
+      <c r="O21" s="24" t="s">
         <v>332</v>
       </c>
       <c r="P21" s="23" t="s">
         <v>333</v>
       </c>
+      <c r="Q21" s="23" t="s">
+        <v>334</v>
+      </c>
     </row>
-    <row r="22" spans="1:16">
-      <c r="A22" s="3" t="s">
-        <v>334</v>
+    <row r="22" spans="1:17">
+      <c r="A22" s="2">
+        <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="8" t="s">
         <v>340</v>
       </c>
       <c r="H22" s="2" t="s">
@@ -5065,10 +5117,10 @@
       <c r="J22" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="K22" s="21" t="s">
+      <c r="K22" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="L22" s="22" t="s">
+      <c r="L22" s="21" t="s">
         <v>345</v>
       </c>
       <c r="M22" s="22" t="s">
@@ -5077,33 +5129,36 @@
       <c r="N22" s="22" t="s">
         <v>347</v>
       </c>
-      <c r="O22" s="23" t="s">
+      <c r="O22" s="22" t="s">
         <v>348</v>
       </c>
       <c r="P22" s="23" t="s">
         <v>349</v>
       </c>
+      <c r="Q22" s="23" t="s">
+        <v>350</v>
+      </c>
     </row>
-    <row r="23" spans="1:16">
-      <c r="A23" s="3" t="s">
-        <v>350</v>
+    <row r="23" spans="1:17">
+      <c r="A23" s="2">
+        <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="12" t="s">
         <v>355</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="8" t="s">
         <v>356</v>
       </c>
       <c r="H23" s="2" t="s">
@@ -5115,58 +5170,61 @@
       <c r="J23" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="K23" s="21" t="s">
+      <c r="K23" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="L23" s="22" t="s">
+      <c r="L23" s="21" t="s">
         <v>361</v>
       </c>
       <c r="M23" s="22" t="s">
         <v>362</v>
       </c>
-      <c r="N23" s="24" t="s">
+      <c r="N23" s="22" t="s">
         <v>363</v>
       </c>
-      <c r="O23" s="23" t="s">
+      <c r="O23" s="24" t="s">
         <v>364</v>
       </c>
-      <c r="P23" s="23"/>
+      <c r="P23" s="23" t="s">
+        <v>365</v>
+      </c>
+      <c r="Q23" s="23"/>
     </row>
-    <row r="24" spans="1:16">
-      <c r="A24" s="4" t="s">
-        <v>365</v>
-      </c>
-      <c r="B24" s="3" t="s">
+    <row r="24" spans="1:17">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="12" t="s">
         <v>368</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="7" t="s">
         <v>369</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="F24" s="12" t="s">
         <v>370</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="17" t="s">
         <v>371</v>
       </c>
-      <c r="H24" s="12" t="s">
+      <c r="H24" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="I24" s="12" t="s">
         <v>373</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="K24" s="21" t="s">
+      <c r="K24" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="L24" s="22" t="s">
+      <c r="L24" s="21" t="s">
         <v>376</v>
       </c>
       <c r="M24" s="22" t="s">
@@ -5175,33 +5233,36 @@
       <c r="N24" s="22" t="s">
         <v>378</v>
       </c>
-      <c r="O24" s="23" t="s">
+      <c r="O24" s="22" t="s">
         <v>379</v>
       </c>
       <c r="P24" s="23" t="s">
         <v>380</v>
       </c>
+      <c r="Q24" s="23" t="s">
+        <v>381</v>
+      </c>
     </row>
-    <row r="25" spans="1:16">
-      <c r="A25" s="4" t="s">
-        <v>381</v>
-      </c>
-      <c r="B25" s="3" t="s">
+    <row r="25" spans="1:17">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="7" t="s">
         <v>385</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="8" t="s">
         <v>387</v>
       </c>
       <c r="H25" s="2" t="s">
@@ -5213,10 +5274,10 @@
       <c r="J25" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="K25" s="21" t="s">
+      <c r="K25" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="L25" s="22" t="s">
+      <c r="L25" s="21" t="s">
         <v>392</v>
       </c>
       <c r="M25" s="22" t="s">
@@ -5225,33 +5286,36 @@
       <c r="N25" s="22" t="s">
         <v>394</v>
       </c>
-      <c r="O25" s="23" t="s">
+      <c r="O25" s="22" t="s">
         <v>395</v>
       </c>
       <c r="P25" s="23" t="s">
         <v>396</v>
       </c>
+      <c r="Q25" s="23" t="s">
+        <v>397</v>
+      </c>
     </row>
-    <row r="26" spans="1:16">
-      <c r="A26" s="4" t="s">
-        <v>397</v>
-      </c>
-      <c r="B26" s="3" t="s">
+    <row r="26" spans="1:17">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="8" t="s">
         <v>403</v>
       </c>
       <c r="H26" s="2" t="s">
@@ -5263,45 +5327,48 @@
       <c r="J26" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="K26" s="21" t="s">
+      <c r="K26" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="L26" s="30" t="s">
+      <c r="L26" s="21" t="s">
         <v>408</v>
       </c>
-      <c r="M26" s="22" t="s">
+      <c r="M26" s="30" t="s">
         <v>409</v>
       </c>
       <c r="N26" s="22" t="s">
         <v>410</v>
       </c>
-      <c r="O26" s="23" t="s">
+      <c r="O26" s="22" t="s">
         <v>411</v>
       </c>
       <c r="P26" s="23" t="s">
         <v>412</v>
       </c>
+      <c r="Q26" s="23" t="s">
+        <v>413</v>
+      </c>
     </row>
-    <row r="27" spans="1:16">
-      <c r="A27" s="4" t="s">
-        <v>413</v>
-      </c>
-      <c r="B27" s="3" t="s">
+    <row r="27" spans="1:17">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="7" t="s">
         <v>417</v>
       </c>
-      <c r="F27" s="17" t="s">
+      <c r="F27" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G27" s="17" t="s">
         <v>419</v>
       </c>
       <c r="H27" s="2" t="s">
@@ -5313,10 +5380,10 @@
       <c r="J27" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="K27" s="21" t="s">
+      <c r="K27" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="L27" s="22" t="s">
+      <c r="L27" s="21" t="s">
         <v>424</v>
       </c>
       <c r="M27" s="22" t="s">
@@ -5325,83 +5392,89 @@
       <c r="N27" s="22" t="s">
         <v>426</v>
       </c>
-      <c r="O27" s="23" t="s">
+      <c r="O27" s="22" t="s">
         <v>427</v>
       </c>
       <c r="P27" s="23" t="s">
         <v>428</v>
       </c>
+      <c r="Q27" s="23" t="s">
+        <v>429</v>
+      </c>
     </row>
-    <row r="28" spans="1:16">
-      <c r="A28" s="4" t="s">
-        <v>429</v>
-      </c>
-      <c r="B28" s="3" t="s">
+    <row r="28" spans="1:17">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="3" t="s">
         <v>431</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="7" t="s">
         <v>433</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="F28" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="8" t="s">
         <v>435</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="I28" s="12" t="s">
+      <c r="I28" s="2" t="s">
         <v>437</v>
       </c>
       <c r="J28" s="12" t="s">
         <v>438</v>
       </c>
-      <c r="K28" s="21" t="s">
+      <c r="K28" s="12" t="s">
         <v>439</v>
       </c>
-      <c r="L28" s="22" t="s">
+      <c r="L28" s="21" t="s">
         <v>440</v>
       </c>
       <c r="M28" s="22" t="s">
         <v>441</v>
       </c>
-      <c r="N28" s="24" t="s">
+      <c r="N28" s="22" t="s">
         <v>442</v>
       </c>
-      <c r="O28" s="23" t="s">
+      <c r="O28" s="24" t="s">
         <v>443</v>
       </c>
       <c r="P28" s="23" t="s">
         <v>444</v>
       </c>
+      <c r="Q28" s="23" t="s">
+        <v>445</v>
+      </c>
     </row>
-    <row r="29" spans="1:16">
-      <c r="A29" s="4" t="s">
-        <v>445</v>
-      </c>
-      <c r="B29" s="3" t="s">
+    <row r="29" spans="1:17">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="3" t="s">
         <v>447</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="7" t="s">
         <v>449</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F29" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="8" t="s">
         <v>451</v>
       </c>
       <c r="H29" s="2" t="s">
@@ -5413,10 +5486,10 @@
       <c r="J29" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="K29" s="21" t="s">
+      <c r="K29" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="L29" s="22" t="s">
+      <c r="L29" s="21" t="s">
         <v>456</v>
       </c>
       <c r="M29" s="22" t="s">
@@ -5425,83 +5498,89 @@
       <c r="N29" s="22" t="s">
         <v>458</v>
       </c>
-      <c r="O29" s="23" t="s">
+      <c r="O29" s="22" t="s">
         <v>459</v>
       </c>
       <c r="P29" s="23" t="s">
         <v>460</v>
       </c>
+      <c r="Q29" s="23" t="s">
+        <v>461</v>
+      </c>
     </row>
-    <row r="30" spans="1:16">
-      <c r="A30" s="4" t="s">
-        <v>461</v>
-      </c>
-      <c r="B30" s="3" t="s">
+    <row r="30" spans="1:17">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>462</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="3" t="s">
         <v>463</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="7" t="s">
         <v>465</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="8" t="s">
         <v>467</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="I30" s="12" t="s">
+      <c r="I30" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="J30" s="12" t="s">
         <v>470</v>
       </c>
-      <c r="K30" s="21" t="s">
+      <c r="K30" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="L30" s="22" t="s">
+      <c r="L30" s="21" t="s">
         <v>472</v>
       </c>
       <c r="M30" s="22" t="s">
         <v>473</v>
       </c>
-      <c r="N30" s="24" t="s">
+      <c r="N30" s="22" t="s">
         <v>474</v>
       </c>
-      <c r="O30" s="23" t="s">
+      <c r="O30" s="24" t="s">
         <v>475</v>
       </c>
       <c r="P30" s="23" t="s">
         <v>476</v>
       </c>
+      <c r="Q30" s="23" t="s">
+        <v>477</v>
+      </c>
     </row>
-    <row r="31" spans="1:16">
-      <c r="A31" s="4" t="s">
-        <v>477</v>
-      </c>
-      <c r="B31" s="3" t="s">
+    <row r="31" spans="1:17">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>478</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="3" t="s">
         <v>479</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" s="7" t="s">
         <v>481</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F31" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" s="8" t="s">
         <v>483</v>
       </c>
       <c r="H31" s="2" t="s">
@@ -5510,13 +5589,13 @@
       <c r="I31" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="J31" s="12" t="s">
+      <c r="J31" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="K31" s="21" t="s">
+      <c r="K31" s="12" t="s">
         <v>487</v>
       </c>
-      <c r="L31" s="22" t="s">
+      <c r="L31" s="21" t="s">
         <v>488</v>
       </c>
       <c r="M31" s="22" t="s">
@@ -5525,33 +5604,36 @@
       <c r="N31" s="22" t="s">
         <v>490</v>
       </c>
-      <c r="O31" s="23" t="s">
+      <c r="O31" s="22" t="s">
         <v>491</v>
       </c>
       <c r="P31" s="23" t="s">
         <v>492</v>
       </c>
+      <c r="Q31" s="23" t="s">
+        <v>493</v>
+      </c>
     </row>
-    <row r="32" spans="1:16">
-      <c r="A32" s="4" t="s">
-        <v>493</v>
-      </c>
-      <c r="B32" s="3" t="s">
+    <row r="32" spans="1:17">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>494</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="3" t="s">
         <v>495</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" s="7" t="s">
         <v>497</v>
       </c>
-      <c r="F32" s="17" t="s">
+      <c r="F32" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G32" s="17" t="s">
         <v>499</v>
       </c>
       <c r="H32" s="2" t="s">
@@ -5560,48 +5642,51 @@
       <c r="I32" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="J32" s="12" t="s">
+      <c r="J32" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="K32" s="21" t="s">
+      <c r="K32" s="12" t="s">
         <v>503</v>
       </c>
-      <c r="L32" s="24" t="s">
+      <c r="L32" s="21" t="s">
         <v>504</v>
       </c>
-      <c r="M32" s="22" t="s">
+      <c r="M32" s="24" t="s">
         <v>505</v>
       </c>
-      <c r="N32" s="29" t="s">
+      <c r="N32" s="22" t="s">
         <v>506</v>
       </c>
-      <c r="O32" s="23" t="s">
+      <c r="O32" s="29" t="s">
         <v>507</v>
       </c>
       <c r="P32" s="23" t="s">
         <v>508</v>
       </c>
+      <c r="Q32" s="23" t="s">
+        <v>509</v>
+      </c>
     </row>
     <row r="33" spans="1:17">
-      <c r="A33" s="4" t="s">
-        <v>509</v>
-      </c>
-      <c r="B33" s="3" t="s">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="3" t="s">
         <v>511</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="7" t="s">
         <v>513</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F33" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G33" s="8" t="s">
         <v>515</v>
       </c>
       <c r="H33" s="2" t="s">
@@ -5613,45 +5698,48 @@
       <c r="J33" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="K33" s="21" t="s">
+      <c r="K33" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="L33" s="22" t="s">
+      <c r="L33" s="21" t="s">
         <v>520</v>
       </c>
       <c r="M33" s="22" t="s">
         <v>521</v>
       </c>
-      <c r="N33" s="24" t="s">
+      <c r="N33" s="22" t="s">
         <v>522</v>
       </c>
-      <c r="O33" s="23" t="s">
+      <c r="O33" s="24" t="s">
         <v>523</v>
       </c>
       <c r="P33" s="23" t="s">
         <v>524</v>
       </c>
+      <c r="Q33" s="23" t="s">
+        <v>525</v>
+      </c>
     </row>
     <row r="34" spans="1:17">
-      <c r="A34" s="4" t="s">
-        <v>525</v>
-      </c>
-      <c r="B34" s="3" t="s">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>526</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="3" t="s">
         <v>527</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="7" t="s">
         <v>529</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="F34" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G34" s="8" t="s">
         <v>531</v>
       </c>
       <c r="H34" s="2" t="s">
@@ -5663,55 +5751,58 @@
       <c r="J34" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="K34" s="21" t="s">
+      <c r="K34" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="L34" s="24" t="s">
+      <c r="L34" s="21" t="s">
         <v>536</v>
       </c>
-      <c r="M34" s="22" t="s">
+      <c r="M34" s="24" t="s">
         <v>537</v>
       </c>
       <c r="N34" s="22" t="s">
         <v>538</v>
       </c>
-      <c r="O34" s="23" t="s">
+      <c r="O34" s="22" t="s">
         <v>539</v>
       </c>
       <c r="P34" s="23" t="s">
         <v>540</v>
       </c>
+      <c r="Q34" s="23" t="s">
+        <v>541</v>
+      </c>
     </row>
     <row r="35" spans="1:17">
-      <c r="A35" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>541</v>
-      </c>
-      <c r="C35" s="2" t="s">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>542</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E35" s="7" t="s">
         <v>544</v>
       </c>
-      <c r="F35" s="8"/>
-      <c r="G35" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>545</v>
       </c>
+      <c r="G35" s="8"/>
       <c r="H35" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="I35" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="K35" s="21" t="s">
+      <c r="K35" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="L35" s="22" t="s">
+      <c r="L35" s="21" t="s">
         <v>549</v>
       </c>
       <c r="M35" s="22" t="s">
@@ -5720,33 +5811,36 @@
       <c r="N35" s="22" t="s">
         <v>551</v>
       </c>
-      <c r="O35" s="28" t="s">
+      <c r="O35" s="22" t="s">
         <v>552</v>
       </c>
-      <c r="P35" s="23" t="s">
+      <c r="P35" s="28" t="s">
         <v>553</v>
+      </c>
+      <c r="Q35" s="23" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="36" spans="1:17">
-      <c r="A36" s="4" t="s">
-        <v>554</v>
-      </c>
-      <c r="B36" s="3" t="s">
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>555</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="12" t="s">
         <v>557</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E36" s="7" t="s">
         <v>558</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="F36" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G36" s="8" t="s">
         <v>560</v>
       </c>
       <c r="H36" s="2" t="s">
@@ -5758,10 +5852,10 @@
       <c r="J36" s="2" t="s">
         <v>563</v>
       </c>
-      <c r="K36" s="21" t="s">
+      <c r="K36" s="2" t="s">
         <v>564</v>
       </c>
-      <c r="L36" s="22" t="s">
+      <c r="L36" s="21" t="s">
         <v>565</v>
       </c>
       <c r="M36" s="22" t="s">
@@ -5770,33 +5864,36 @@
       <c r="N36" s="22" t="s">
         <v>567</v>
       </c>
-      <c r="O36" s="23" t="s">
+      <c r="O36" s="22" t="s">
         <v>568</v>
       </c>
       <c r="P36" s="23" t="s">
         <v>569</v>
       </c>
+      <c r="Q36" s="23" t="s">
+        <v>570</v>
+      </c>
     </row>
     <row r="37" spans="1:17">
-      <c r="A37" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>570</v>
-      </c>
-      <c r="C37" s="2" t="s">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>571</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E37" s="7" t="s">
         <v>573</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="F37" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G37" s="8" t="s">
         <v>575</v>
       </c>
       <c r="H37" s="2" t="s">
@@ -5808,45 +5905,48 @@
       <c r="J37" s="2" t="s">
         <v>578</v>
       </c>
-      <c r="K37" s="21" t="s">
+      <c r="K37" s="2" t="s">
         <v>579</v>
       </c>
-      <c r="L37" s="22" t="s">
+      <c r="L37" s="21" t="s">
         <v>580</v>
       </c>
       <c r="M37" s="22" t="s">
         <v>581</v>
       </c>
-      <c r="N37" s="24" t="s">
+      <c r="N37" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="O37" s="23" t="s">
+      <c r="O37" s="24" t="s">
         <v>583</v>
       </c>
       <c r="P37" s="23" t="s">
         <v>584</v>
       </c>
+      <c r="Q37" s="23" t="s">
+        <v>585</v>
+      </c>
     </row>
     <row r="38" spans="1:17">
-      <c r="A38" s="4" t="s">
-        <v>585</v>
-      </c>
-      <c r="B38" s="3" t="s">
+      <c r="A38" s="2">
+        <v>37</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>586</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="3" t="s">
         <v>587</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E38" s="7" t="s">
         <v>589</v>
       </c>
-      <c r="F38" s="8" t="s">
+      <c r="F38" s="2" t="s">
         <v>590</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G38" s="8" t="s">
         <v>591</v>
       </c>
       <c r="H38" s="2" t="s">
@@ -5855,13 +5955,13 @@
       <c r="I38" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="J38" s="12" t="s">
+      <c r="J38" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="K38" s="21" t="s">
+      <c r="K38" s="12" t="s">
         <v>595</v>
       </c>
-      <c r="L38" s="22" t="s">
+      <c r="L38" s="21" t="s">
         <v>596</v>
       </c>
       <c r="M38" s="22" t="s">
@@ -5870,33 +5970,36 @@
       <c r="N38" s="22" t="s">
         <v>598</v>
       </c>
-      <c r="O38" s="23" t="s">
+      <c r="O38" s="22" t="s">
         <v>599</v>
       </c>
       <c r="P38" s="23" t="s">
         <v>600</v>
       </c>
+      <c r="Q38" s="23" t="s">
+        <v>601</v>
+      </c>
     </row>
     <row r="39" spans="1:17">
-      <c r="A39" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>601</v>
-      </c>
-      <c r="C39" s="2" t="s">
+      <c r="A39" s="2">
+        <v>38</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>602</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="D39" s="2" t="s">
         <v>603</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E39" s="13" t="s">
         <v>604</v>
       </c>
-      <c r="F39" s="14" t="s">
+      <c r="F39" s="2" t="s">
         <v>605</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="G39" s="14" t="s">
         <v>606</v>
       </c>
       <c r="H39" s="2" t="s">
@@ -5908,111 +6011,116 @@
       <c r="J39" s="2" t="s">
         <v>609</v>
       </c>
-      <c r="K39" s="21" t="s">
+      <c r="K39" s="2" t="s">
         <v>610</v>
       </c>
-      <c r="L39" s="22" t="s">
+      <c r="L39" s="21" t="s">
         <v>611</v>
       </c>
       <c r="M39" s="22" t="s">
         <v>612</v>
       </c>
-      <c r="N39" s="29" t="s">
+      <c r="N39" s="22" t="s">
         <v>613</v>
       </c>
-      <c r="O39" s="23" t="s">
+      <c r="O39" s="29" t="s">
         <v>614</v>
       </c>
       <c r="P39" s="23" t="s">
         <v>615</v>
       </c>
+      <c r="Q39" s="23" t="s">
+        <v>616</v>
+      </c>
     </row>
-    <row r="40" spans="1:17" s="32" customFormat="1">
-      <c r="A40" s="33" t="s">
-        <v>616</v>
-      </c>
-      <c r="B40" s="34" t="s">
+    <row r="40" spans="1:17">
+      <c r="A40" s="2">
+        <v>39</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>617</v>
       </c>
-      <c r="C40" s="32" t="s">
+      <c r="C40" s="3" t="s">
         <v>618</v>
       </c>
-      <c r="D40" s="35" t="s">
+      <c r="D40" s="2" t="s">
         <v>619</v>
       </c>
-      <c r="E40" s="32" t="s">
+      <c r="E40" s="7" t="s">
         <v>620</v>
       </c>
-      <c r="F40" s="36" t="s">
+      <c r="F40" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="G40" s="32" t="s">
+      <c r="G40" s="8" t="s">
         <v>622</v>
       </c>
-      <c r="H40" s="32" t="s">
+      <c r="H40" s="2" t="s">
         <v>623</v>
       </c>
-      <c r="I40" s="32" t="s">
+      <c r="I40" s="2" t="s">
         <v>624</v>
       </c>
-      <c r="J40" s="32" t="s">
+      <c r="J40" s="2" t="s">
         <v>625</v>
       </c>
-      <c r="K40" s="37" t="s">
+      <c r="K40" s="2" t="s">
         <v>626</v>
       </c>
-      <c r="L40" s="38" t="s">
+      <c r="L40" s="21" t="s">
         <v>627</v>
       </c>
-      <c r="M40" s="39" t="s">
+      <c r="M40" s="22" t="s">
         <v>628</v>
       </c>
-      <c r="N40" s="38" t="s">
+      <c r="N40" s="32" t="s">
         <v>629</v>
       </c>
-      <c r="O40" s="40" t="s">
+      <c r="O40" s="22" t="s">
         <v>630</v>
       </c>
-      <c r="P40" s="40" t="s">
+      <c r="P40" s="23" t="s">
         <v>631</v>
       </c>
-      <c r="Q40" s="36"/>
+      <c r="Q40" s="23" t="s">
+        <v>632</v>
+      </c>
     </row>
     <row r="41" spans="1:17">
-      <c r="A41" s="4" t="s">
-        <v>632</v>
-      </c>
-      <c r="B41" s="3" t="s">
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>633</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="3" t="s">
         <v>634</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="2" t="s">
         <v>635</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E41" s="7" t="s">
         <v>636</v>
       </c>
-      <c r="F41" s="8" t="s">
+      <c r="F41" s="2" t="s">
         <v>637</v>
       </c>
-      <c r="G41" s="12" t="s">
+      <c r="G41" s="8" t="s">
         <v>638</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="H41" s="12" t="s">
         <v>639</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="J41" s="12" t="s">
+      <c r="J41" s="2" t="s">
         <v>641</v>
       </c>
-      <c r="K41" s="21" t="s">
+      <c r="K41" s="12" t="s">
         <v>642</v>
       </c>
-      <c r="L41" s="22" t="s">
+      <c r="L41" s="21" t="s">
         <v>643</v>
       </c>
       <c r="M41" s="22" t="s">
@@ -6021,33 +6129,36 @@
       <c r="N41" s="22" t="s">
         <v>645</v>
       </c>
-      <c r="O41" s="23" t="s">
+      <c r="O41" s="22" t="s">
         <v>646</v>
       </c>
       <c r="P41" s="23" t="s">
         <v>647</v>
       </c>
+      <c r="Q41" s="23" t="s">
+        <v>648</v>
+      </c>
     </row>
     <row r="42" spans="1:17">
-      <c r="A42" s="4" t="s">
-        <v>648</v>
-      </c>
-      <c r="B42" s="3" t="s">
+      <c r="A42" s="2">
+        <v>41</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>649</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="3" t="s">
         <v>650</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="2" t="s">
         <v>651</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E42" s="7" t="s">
         <v>652</v>
       </c>
-      <c r="F42" s="8" t="s">
+      <c r="F42" s="2" t="s">
         <v>653</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="G42" s="8" t="s">
         <v>654</v>
       </c>
       <c r="H42" s="2" t="s">
@@ -6056,48 +6167,51 @@
       <c r="I42" s="2" t="s">
         <v>656</v>
       </c>
-      <c r="J42" s="12" t="s">
+      <c r="J42" s="2" t="s">
         <v>657</v>
       </c>
-      <c r="K42" s="21" t="s">
+      <c r="K42" s="12" t="s">
         <v>658</v>
       </c>
-      <c r="L42" s="24" t="s">
+      <c r="L42" s="21" t="s">
         <v>659</v>
       </c>
-      <c r="M42" s="22" t="s">
+      <c r="M42" s="24" t="s">
         <v>660</v>
       </c>
       <c r="N42" s="22" t="s">
         <v>661</v>
       </c>
-      <c r="O42" s="23" t="s">
+      <c r="O42" s="22" t="s">
         <v>662</v>
       </c>
       <c r="P42" s="23" t="s">
         <v>663</v>
       </c>
+      <c r="Q42" s="23" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="43" spans="1:17">
-      <c r="A43" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>664</v>
-      </c>
-      <c r="C43" s="2" t="s">
+      <c r="A43" s="2">
+        <v>42</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>665</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="2" t="s">
         <v>666</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="E43" s="7" t="s">
         <v>667</v>
       </c>
-      <c r="F43" s="8" t="s">
+      <c r="F43" s="2" t="s">
         <v>668</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="G43" s="8" t="s">
         <v>669</v>
       </c>
       <c r="H43" s="2" t="s">
@@ -6106,48 +6220,51 @@
       <c r="I43" s="2" t="s">
         <v>671</v>
       </c>
-      <c r="J43" s="16" t="s">
+      <c r="J43" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="K43" s="21" t="s">
+      <c r="K43" s="16" t="s">
         <v>673</v>
       </c>
-      <c r="L43" s="26" t="s">
+      <c r="L43" s="21" t="s">
         <v>674</v>
       </c>
-      <c r="M43" s="31" t="s">
+      <c r="M43" s="26" t="s">
         <v>675</v>
       </c>
-      <c r="N43" s="22" t="s">
+      <c r="N43" s="31" t="s">
         <v>676</v>
       </c>
-      <c r="O43" s="28" t="s">
+      <c r="O43" s="22" t="s">
         <v>677</v>
       </c>
       <c r="P43" s="28" t="s">
         <v>678</v>
       </c>
+      <c r="Q43" s="28" t="s">
+        <v>679</v>
+      </c>
     </row>
     <row r="44" spans="1:17">
-      <c r="A44" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>679</v>
-      </c>
-      <c r="C44" s="2" t="s">
+      <c r="A44" s="2">
+        <v>43</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>680</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="2" t="s">
         <v>681</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E44" s="7" t="s">
         <v>682</v>
       </c>
-      <c r="F44" s="8" t="s">
+      <c r="F44" s="2" t="s">
         <v>683</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="G44" s="8" t="s">
         <v>684</v>
       </c>
       <c r="H44" s="2" t="s">
@@ -6156,13 +6273,13 @@
       <c r="I44" s="2" t="s">
         <v>686</v>
       </c>
-      <c r="J44" s="12" t="s">
+      <c r="J44" s="2" t="s">
         <v>687</v>
       </c>
-      <c r="K44" s="21" t="s">
+      <c r="K44" s="12" t="s">
         <v>688</v>
       </c>
-      <c r="L44" s="22" t="s">
+      <c r="L44" s="21" t="s">
         <v>689</v>
       </c>
       <c r="M44" s="22" t="s">
@@ -6171,33 +6288,36 @@
       <c r="N44" s="22" t="s">
         <v>691</v>
       </c>
-      <c r="O44" s="23" t="s">
+      <c r="O44" s="22" t="s">
         <v>692</v>
       </c>
       <c r="P44" s="23" t="s">
         <v>693</v>
       </c>
+      <c r="Q44" s="23" t="s">
+        <v>694</v>
+      </c>
     </row>
     <row r="45" spans="1:17">
-      <c r="A45" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>694</v>
-      </c>
-      <c r="C45" s="2" t="s">
+      <c r="A45" s="2">
+        <v>44</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>695</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="2" t="s">
         <v>696</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="E45" s="7" t="s">
         <v>697</v>
       </c>
-      <c r="F45" s="8" t="s">
+      <c r="F45" s="2" t="s">
         <v>698</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="G45" s="8" t="s">
         <v>699</v>
       </c>
       <c r="H45" s="2" t="s">
@@ -6209,10 +6329,10 @@
       <c r="J45" s="2" t="s">
         <v>702</v>
       </c>
-      <c r="K45" s="21" t="s">
+      <c r="K45" s="2" t="s">
         <v>703</v>
       </c>
-      <c r="L45" s="22" t="s">
+      <c r="L45" s="21" t="s">
         <v>704</v>
       </c>
       <c r="M45" s="22" t="s">
@@ -6221,33 +6341,36 @@
       <c r="N45" s="22" t="s">
         <v>706</v>
       </c>
-      <c r="O45" s="23" t="s">
+      <c r="O45" s="22" t="s">
         <v>707</v>
       </c>
       <c r="P45" s="23" t="s">
         <v>708</v>
       </c>
+      <c r="Q45" s="23" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="46" spans="1:17">
-      <c r="A46" s="4" t="s">
-        <v>709</v>
-      </c>
-      <c r="B46" s="3" t="s">
+      <c r="A46" s="2">
+        <v>45</v>
+      </c>
+      <c r="B46" s="4" t="s">
         <v>710</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="3" t="s">
         <v>711</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D46" s="2" t="s">
         <v>712</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="E46" s="7" t="s">
         <v>713</v>
       </c>
-      <c r="F46" s="8" t="s">
+      <c r="F46" s="2" t="s">
         <v>714</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="G46" s="8" t="s">
         <v>715</v>
       </c>
       <c r="H46" s="2" t="s">
@@ -6259,10 +6382,10 @@
       <c r="J46" s="2" t="s">
         <v>718</v>
       </c>
-      <c r="K46" s="21" t="s">
+      <c r="K46" s="2" t="s">
         <v>719</v>
       </c>
-      <c r="L46" s="22" t="s">
+      <c r="L46" s="21" t="s">
         <v>720</v>
       </c>
       <c r="M46" s="22" t="s">
@@ -6271,40 +6394,31 @@
       <c r="N46" s="22" t="s">
         <v>722</v>
       </c>
-      <c r="O46" s="23" t="s">
+      <c r="O46" s="22" t="s">
         <v>723</v>
       </c>
-      <c r="P46" s="41" t="s">
+      <c r="P46" s="23" t="s">
         <v>724</v>
+      </c>
+      <c r="Q46" s="34" t="s">
+        <v>725</v>
       </c>
     </row>
     <row r="47" spans="1:17">
-      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
     </row>
     <row r="48" spans="1:17">
-      <c r="E48"/>
       <c r="F48"/>
       <c r="G48"/>
+      <c r="H48"/>
     </row>
-    <row r="49" spans="4:8"/>
-    <row r="50" spans="4:8"/>
-    <row r="52" spans="4:8">
-      <c r="D52" s="32"/>
-    </row>
-    <row r="53" spans="4:8">
-      <c r="D53" s="32"/>
-      <c r="H53" s="32"/>
-    </row>
-    <row r="54" spans="4:8">
-      <c r="D54" s="32"/>
-    </row>
-    <row r="55" spans="4:8" ht="15" customHeight="1">
-      <c r="D55" s="32"/>
-    </row>
-    <row r="56" spans="4:8">
-      <c r="D56" s="32"/>
-    </row>
-    <row r="58" spans="4:8"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="56"/>
+    <row r="58"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>